<commit_message>
DEAV interface implemented to be consistent with BR use
</commit_message>
<xml_diff>
--- a/data-enrichment-and-validation/doc/Foodex validation_changes.xlsx
+++ b/data-enrichment-and-validation/doc/Foodex validation_changes.xlsx
@@ -258,24 +258,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -301,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -318,9 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -328,8 +313,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,7 +677,7 @@
   <dimension ref="C2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +686,7 @@
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="58.28515625" customWidth="1"/>
     <col min="6" max="6" width="45.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20" style="7" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -718,7 +703,7 @@
       <c r="F2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -735,7 +720,7 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -752,7 +737,7 @@
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -769,7 +754,7 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -786,7 +771,7 @@
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -803,7 +788,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -820,7 +805,7 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -837,7 +822,7 @@
       <c r="F9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -854,7 +839,7 @@
       <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -862,7 +847,7 @@
       <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -871,7 +856,7 @@
       <c r="F11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -879,8 +864,8 @@
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>30</v>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>32</v>
@@ -888,7 +873,7 @@
       <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -896,7 +881,7 @@
       <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -905,7 +890,7 @@
       <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -913,7 +898,7 @@
       <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -922,7 +907,7 @@
       <c r="F14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -930,7 +915,7 @@
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -939,7 +924,7 @@
       <c r="F15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -947,7 +932,7 @@
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -956,7 +941,7 @@
       <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -964,7 +949,7 @@
       <c r="C17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -973,7 +958,7 @@
       <c r="F17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -981,7 +966,7 @@
       <c r="C18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -990,7 +975,7 @@
       <c r="F18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -998,7 +983,7 @@
       <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1007,7 +992,7 @@
       <c r="F19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1015,7 +1000,7 @@
       <c r="C20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1024,7 +1009,7 @@
       <c r="F20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1032,7 +1017,7 @@
       <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1041,7 +1026,7 @@
       <c r="F21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>